<commit_message>
Add Vlad to Table file
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159392DC-FA13-4CD3-AB9F-02B771E6C4F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B118C3-0B7B-469C-9BBA-DA59D2EDB47C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>ID</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Galyna</t>
+  </si>
+  <si>
+    <t>Vlad</t>
   </si>
 </sst>
 </file>
@@ -349,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -381,6 +384,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>333</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Guest to Table file
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B118C3-0B7B-469C-9BBA-DA59D2EDB47C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155046E4-3EB6-4DD1-AAB1-94069075D399}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ID</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Vlad</t>
+  </si>
+  <si>
+    <t>Guest</t>
   </si>
 </sst>
 </file>
@@ -352,10 +355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,6 +395,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>444</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add NewBorn to Table file
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B118C3-0B7B-469C-9BBA-DA59D2EDB47C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DCAEB4-0228-4EBF-8227-7853C2355076}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ID</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Vlad</t>
+  </si>
+  <si>
+    <t>NewBorn</t>
   </si>
 </sst>
 </file>
@@ -352,10 +355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,6 +395,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>444</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Alter NewBorn to Table file
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155046E4-3EB6-4DD1-AAB1-94069075D399}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7AF654-9AC5-4958-98A0-45FD8E40CFC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -355,10 +355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,11 +395,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>444</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Compose NewBorn and Guest to Table file
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7AF654-9AC5-4958-98A0-45FD8E40CFC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D36A4E-86CC-41F0-A863-86A57B45B40F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ID</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Guest</t>
+  </si>
+  <si>
+    <t>NewBorn</t>
   </si>
 </sst>
 </file>
@@ -358,7 +361,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,6 +398,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>444</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>444</v>

</xml_diff>

<commit_message>
Add Vova to Table.xml
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D36A4E-86CC-41F0-A863-86A57B45B40F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F3340D-BE7F-4537-BAAD-760F51F0DC4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ID</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>NewBorn</t>
+  </si>
+  <si>
+    <t>Vova</t>
   </si>
 </sst>
 </file>
@@ -358,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,6 +417,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>555</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>